<commit_message>
Update fuel properties spec and add dash design doc
Replaces FuelProperties_Spec.csv with a new FuelProperties_Spec.xlsx file, reflecting a migration to spreadsheet format. Adds Dash Design.pptx and updates Codex_Task_Backlog-20251212.xlsx. Removes the outdated CSV specification.
</commit_message>
<xml_diff>
--- a/Docs/Codex_Task_Backlog-20251212.xlsx
+++ b/Docs/Codex_Task_Backlog-20251212.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Github\LalaLaunchPlugin\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D9C82E-C098-4543-A9AD-8F53E5BE318B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382E10A8-4F42-4033-979C-9B41A1BBF9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="0" windowWidth="26325" windowHeight="13995" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasking Order" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="296">
   <si>
     <t>ID</t>
   </si>
@@ -1306,6 +1306,18 @@
   </si>
   <si>
     <t>LalaLaunch.Fuel.Pit.StopsRequiredToEnd needs investigating because it shows stop required after final stop and enough fuel til end of race</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>Create a full fuel-properties technical spec</t>
+  </si>
+  <si>
+    <t>Produce a single, authoritative document that lists every fuel-related property our plugin exposes, and for each one provides: (1) unit, (2) calculation/formula, (3) input sources (SimHub telemetry properties + internal state), (4) update timing, and (5) code locations.</t>
+  </si>
+  <si>
+    <t>Document created</t>
   </si>
 </sst>
 </file>
@@ -1929,7 +1941,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,9 +2969,27 @@
         <v>291</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>220</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update documentation files and add fuel properties spec
Updated Codex task backlog and Dash Design presentation files. Added new FuelProperties_Spec (version 1).xlsx to the documentation.
</commit_message>
<xml_diff>
--- a/Docs/Codex_Task_Backlog-20251212.xlsx
+++ b/Docs/Codex_Task_Backlog-20251212.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382E10A8-4F42-4033-979C-9B41A1BBF9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{901604C7-9458-4450-90E3-605A9627E20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,11 +20,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$G$20</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="301">
   <si>
     <t>ID</t>
   </si>
@@ -1318,6 +1319,27 @@
   </si>
   <si>
     <t>Document created</t>
+  </si>
+  <si>
+    <t>Stabilise dash-facing fuel properties by enforcing gated pace inputs, filtering outliers, and adding optional smoothed variants (no behaviour regressions).</t>
+  </si>
+  <si>
+    <t>Reduce jitter/jumping in dash-facing fuel/pit properties by ensuring projection uses our gated averages (last 5 clean laps / stint avg) instead of any instantaneous sources, filtering telemetry outliers, and providing optional smoothed versions of key properties. Do NOT change the meaning of existing properties; add smoothed variants where needed.</t>
+  </si>
+  <si>
+    <t>In replay/live, key dash-facing values (laps remaining, deltas, total needed) no longer “jump” due to instantaneous lap/leader telemetry spikes.
+Leader lap time glitches (e.g. 1–5s) do not corrupt leader pace or downstream calculations.
+LiveLapsRemainingInRace uses gated pace sources whenever available (verified via log/source selection).
+Existing Fuel tab strategy and existing raw properties remain unchanged in meaning and are not destabilised.
+Smoothed properties appear in SimHub property browser and behave as expected (stable yet responsive).</t>
+  </si>
+  <si>
+    <t>As per the title and description</t>
+  </si>
+  <si>
+    <t>Enforced timed-race lap-time selection priority (stint average → last 5 → profile baseline → estimator) with gated logging and kept projections anchored to the strategy-provided after-zero allowance.
+Filtered leader lap outliers, falling back to the existing leader average when telemetry spikes occur and preventing fallback samples from polluting the rolling window.
+Added EMA-smoothed dash-facing fuel and pit properties, wiring session/pit change resets and exposing the new smoothed values alongside existing raw outputs.</t>
   </si>
 </sst>
 </file>
@@ -1938,10 +1960,10 @@
   <dimension ref="A1:N82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomRight" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,13 +2982,16 @@
         <v>219</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>290</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>291</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -2992,9 +3017,33 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>221</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix overall leader validity logic in LalaLaunch.cs
Refactors the logic for setting OverallLeaderHasFinishedValid to ensure it reflects whether the overall leader index is valid, regardless of session type. This clarifies the meaning of the validity flag and improves code readability.
</commit_message>
<xml_diff>
--- a/Docs/Codex_Task_Backlog-20251212.xlsx
+++ b/Docs/Codex_Task_Backlog-20251212.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{901604C7-9458-4450-90E3-605A9627E20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81D5F61-AC8A-401E-A835-2DD795BE899C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasking Order" sheetId="2" r:id="rId1"/>
@@ -20,12 +20,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$G$20</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="305">
   <si>
     <t>ID</t>
   </si>
@@ -344,9 +343,6 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Dependent on other Task</t>
-  </si>
-  <si>
     <t>Codebase / Structure / Cleanup</t>
   </si>
   <si>
@@ -924,9 +920,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Tried to save planner data to new preset but after hitting save there is an issue where the new profile does not show in the list. When checking also on the fuel tab, the preset name does change there but also does not show in the combo box. I tried to go back to the preset tab but the tab is not loading when clicked on!</t>
   </si>
   <si>
     <t>Initial test show time counting up over multiple lapped counts which is incorrect. Will create new task.
@@ -1341,12 +1334,30 @@
 Filtered leader lap outliers, falling back to the existing leader average when telemetry spikes occur and preventing fallback samples from polluting the rolling window.
 Added EMA-smoothed dash-facing fuel and pit properties, wiring session/pit change resets and exposing the new smoothed values alongside existing raw outputs.</t>
   </si>
+  <si>
+    <t>Has Issues</t>
+  </si>
+  <si>
+    <t>Still requires testing in wet session</t>
+  </si>
+  <si>
+    <t>Waiting tests</t>
+  </si>
+  <si>
+    <t>Needs further investigation - Think I saw the Fuel Burn text box and choices look stale and not picking up new profile. Will need to test</t>
+  </si>
+  <si>
+    <t>Needs further work. I noticed that with live source selected at session start it correctly uses the profile value while live average data is mined and updated. However, it never changes the Lap time text box to live once available unless I toggle to profile then back to live. Small annoying issue that will need fixing.</t>
+  </si>
+  <si>
+    <t>This is also mentioned in LALA-38 and can be merged to that task.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1391,6 +1402,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1407,8 +1425,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1436,10 +1453,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1456,11 +1474,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1960,10 +1982,10 @@
   <dimension ref="A1:N82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2007,16 +2029,16 @@
         <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>63</v>
@@ -2048,10 +2070,10 @@
         <v>89</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>58</v>
@@ -2083,7 +2105,7 @@
         <v>60</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>62</v>
@@ -2106,16 +2128,16 @@
         <v>41</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>59</v>
@@ -2132,31 +2154,31 @@
         <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>62</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>88</v>
@@ -2188,7 +2210,7 @@
         <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>89</v>
@@ -2220,10 +2242,10 @@
         <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>93</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -2249,7 +2271,7 @@
         <v>89</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>61</v>
@@ -2263,28 +2285,28 @@
         <v>92</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L9" s="3"/>
     </row>
@@ -2314,13 +2336,13 @@
         <v>65</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
@@ -2340,7 +2362,7 @@
         <v>72</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>61</v>
@@ -2349,10 +2371,10 @@
         <v>73</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="285" x14ac:dyDescent="0.25">
@@ -2372,36 +2394,37 @@
         <v>75</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>76</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>204</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:14" ht="405" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
@@ -2421,7 +2444,7 @@
         <v>78</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>62</v>
@@ -2430,10 +2453,13 @@
         <v>79</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
@@ -2456,16 +2482,16 @@
         <v>86</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>82</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="405" x14ac:dyDescent="0.25">
@@ -2476,22 +2502,22 @@
         <v>84</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
@@ -2505,22 +2531,22 @@
         <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
@@ -2534,28 +2560,28 @@
         <v>37</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
@@ -2569,25 +2595,28 @@
         <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>62</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="390" x14ac:dyDescent="0.25">
@@ -2607,24 +2636,27 @@
         <v>69</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>62</v>
+        <v>299</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>70</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>87</v>
@@ -2633,179 +2665,209 @@
         <v>67</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>58</v>
+        <v>299</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>151</v>
+      <c r="K21" s="7" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>154</v>
+      <c r="G22" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>167</v>
+      <c r="G23" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>169</v>
+      <c r="G24" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>173</v>
+      <c r="G25" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>177</v>
+      <c r="G26" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>181</v>
+      <c r="G27" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>184</v>
+      <c r="F28" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>92</v>
@@ -2814,204 +2876,204 @@
         <v>37</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="K32" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>61</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
@@ -3019,241 +3081,241 @@
     </row>
     <row r="40" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="G40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>